<commit_message>
updated with co-optimization of H2 and Power system
</commit_message>
<xml_diff>
--- a/Python/Data/NewPlantData/NewTechFramework.xlsx
+++ b/Python/Data/NewPlantData/NewTechFramework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atpha\Documents\Postdocs\Projects\NETs\Model\Python\Data\NewPlantData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atpha\Documents\Postdocs\Projects\MacroCEM\Model\Python\Data\NewPlantData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92A521C-0CA7-410C-99D7-50292C24FE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08351A7F-D53B-4EDE-AA9B-82496BE9E597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="360" windowWidth="19335" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewTechFramework" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="78">
   <si>
     <t>PlantType</t>
   </si>
@@ -187,9 +187,6 @@
     <t>Hydrogen</t>
   </si>
   <si>
-    <t>hydrogen</t>
-  </si>
-  <si>
     <t>CCS</t>
   </si>
   <si>
@@ -212,6 +209,51 @@
   </si>
   <si>
     <t>atb</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>SMR</t>
+  </si>
+  <si>
+    <t>SMR CCS</t>
+  </si>
+  <si>
+    <t>Electrolyzer</t>
+  </si>
+  <si>
+    <t>Fuel Cell</t>
+  </si>
+  <si>
+    <t>H2 Turbine</t>
+  </si>
+  <si>
+    <t>fuel_cell</t>
+  </si>
+  <si>
+    <t>H2_turbine</t>
+  </si>
+  <si>
+    <t>electrolyzer</t>
+  </si>
+  <si>
+    <t>h2_storage</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>h2toelectricity</t>
+  </si>
+  <si>
+    <t>FuelCell</t>
+  </si>
+  <si>
+    <t>H2Turbine</t>
   </si>
 </sst>
 </file>
@@ -701,8 +743,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1024,16 +1067,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
@@ -1129,7 +1172,7 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -1137,7 +1180,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -1191,7 +1234,7 @@
         <v>30</v>
       </c>
       <c r="X2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -1199,7 +1242,7 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
@@ -1253,7 +1296,7 @@
         <v>30</v>
       </c>
       <c r="X3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1261,7 +1304,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -1315,7 +1358,7 @@
         <v>30</v>
       </c>
       <c r="X4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1323,7 +1366,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -1377,7 +1420,7 @@
         <v>30</v>
       </c>
       <c r="X5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1385,7 +1428,7 @@
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
@@ -1439,7 +1482,7 @@
         <v>30</v>
       </c>
       <c r="X6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -1447,7 +1490,7 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
@@ -1509,7 +1552,7 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
@@ -1566,7 +1609,7 @@
         <v>30</v>
       </c>
       <c r="X8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1574,7 +1617,7 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
         <v>48</v>
@@ -1631,7 +1674,7 @@
         <v>30</v>
       </c>
       <c r="X9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1639,7 +1682,7 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
@@ -1698,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -1706,7 +1749,7 @@
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -1763,6 +1806,364 @@
       </c>
       <c r="X11" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12">
+        <v>80</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="K12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>40</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>30</v>
+      </c>
+      <c r="R12" t="s">
+        <v>30</v>
+      </c>
+      <c r="S12" t="s">
+        <v>30</v>
+      </c>
+      <c r="T12" t="s">
+        <v>30</v>
+      </c>
+      <c r="U12" t="s">
+        <v>30</v>
+      </c>
+      <c r="V12" t="s">
+        <v>30</v>
+      </c>
+      <c r="W12" t="s">
+        <v>30</v>
+      </c>
+      <c r="X12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13">
+        <v>9170</v>
+      </c>
+      <c r="K13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>20000</v>
+      </c>
+      <c r="O13">
+        <v>25</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>30</v>
+      </c>
+      <c r="R13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S13" t="s">
+        <v>30</v>
+      </c>
+      <c r="U13" t="s">
+        <v>30</v>
+      </c>
+      <c r="V13" t="s">
+        <v>30</v>
+      </c>
+      <c r="W13" t="s">
+        <v>30</v>
+      </c>
+      <c r="X13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14">
+        <v>9170</v>
+      </c>
+      <c r="K14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>2000</v>
+      </c>
+      <c r="O14">
+        <v>25</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>30</v>
+      </c>
+      <c r="R14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S14" t="s">
+        <v>30</v>
+      </c>
+      <c r="U14" t="s">
+        <v>30</v>
+      </c>
+      <c r="V14" t="s">
+        <v>30</v>
+      </c>
+      <c r="W14" t="s">
+        <v>30</v>
+      </c>
+      <c r="X14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15">
+        <v>2000</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>30</v>
+      </c>
+      <c r="R15" t="s">
+        <v>30</v>
+      </c>
+      <c r="S15" t="s">
+        <v>30</v>
+      </c>
+      <c r="U15" t="s">
+        <v>30</v>
+      </c>
+      <c r="V15" t="s">
+        <v>30</v>
+      </c>
+      <c r="W15" t="s">
+        <v>30</v>
+      </c>
+      <c r="X15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>30</v>
+      </c>
+      <c r="R16" t="s">
+        <v>30</v>
+      </c>
+      <c r="S16" t="s">
+        <v>30</v>
+      </c>
+      <c r="U16" t="s">
+        <v>30</v>
+      </c>
+      <c r="V16" t="s">
+        <v>30</v>
+      </c>
+      <c r="W16" t="s">
+        <v>30</v>
+      </c>
+      <c r="X16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17">
+        <v>240</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>25</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>30</v>
+      </c>
+      <c r="R17" t="s">
+        <v>30</v>
+      </c>
+      <c r="S17" t="s">
+        <v>30</v>
+      </c>
+      <c r="U17" t="s">
+        <v>30</v>
+      </c>
+      <c r="V17" t="s">
+        <v>30</v>
+      </c>
+      <c r="W17" t="s">
+        <v>30</v>
+      </c>
+      <c r="X17" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>